<commit_message>
problem 1 comment (#16)
Co-authored-by: Eric Zeng <ericzeng@Erics-MBP.lan>
</commit_message>
<xml_diff>
--- a/HW4/hw4_9821_fall2023.xlsx
+++ b/HW4/hw4_9821_fall2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericzeng/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericzeng/Documents/numerical-method-for-finance/MTH9821-numerical-method-for-financial-engineering/HW4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7088F44-661F-5E48-92D5-F06735DE2D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEAF974-EE61-EC4E-8F17-70C9E512D1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="2060" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7400" yWindow="4600" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem 1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="38">
   <si>
     <t>Trinomial Tree Methods for American Options</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>In order of convergence speed: TBSR, TBS, and standard trinomial trees.</t>
+  </si>
+  <si>
+    <t>All three methods converge linearly, and TBSR also converges  quadratically but not very fast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greeks converge faster than the valuations. </t>
   </si>
 </sst>
 </file>
@@ -569,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2426,7 +2432,9 @@
       <c r="Z44" s="4"/>
     </row>
     <row r="45" spans="1:26" ht="13">
-      <c r="A45" s="7"/>
+      <c r="A45" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -2454,6 +2462,9 @@
       <c r="Z45" s="4"/>
     </row>
     <row r="46" spans="1:26" ht="13">
+      <c r="A46" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>

</xml_diff>